<commit_message>
Final touches on MOC; now more resilient and accepts different inputs.
</commit_message>
<xml_diff>
--- a/moc_data.xlsx
+++ b/moc_data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD02359-3765-4F58-A552-6D48D2270956}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +331,184 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>53.63194324576201</v>
+      </c>
+      <c r="B2">
+        <v>59.613313518171438</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>78.486691304574578</v>
+      </c>
+      <c r="B3">
+        <v>72.530028314322806</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>94.918730416448554</v>
+      </c>
+      <c r="B4">
+        <v>80.294763843209921</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>111.79351904740416</v>
+      </c>
+      <c r="B5">
+        <v>87.754027900942958</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>129.7956344149467</v>
+      </c>
+      <c r="B6">
+        <v>95.174652557836396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>149.37001427553867</v>
+      </c>
+      <c r="B7">
+        <v>102.67154217157351</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>170.8932301192836</v>
+      </c>
+      <c r="B8">
+        <v>110.29809349679101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>194.73311864238482</v>
+      </c>
+      <c r="B9">
+        <v>118.07452690361883</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>221.27723852371085</v>
+      </c>
+      <c r="B10">
+        <v>125.99813816483909</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>250.9507883081364</v>
+      </c>
+      <c r="B11">
+        <v>134.04661829440482</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>284.23093220033189</v>
+      </c>
+      <c r="B12">
+        <v>142.17801678043591</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>321.66042839806977</v>
+      </c>
+      <c r="B13">
+        <v>150.32863238924617</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>363.86205656024242</v>
+      </c>
+      <c r="B14">
+        <v>158.40926842420325</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>411.55483002827003</v>
+      </c>
+      <c r="B15">
+        <v>166.29990987215484</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>465.57281656215304</v>
+      </c>
+      <c r="B16">
+        <v>173.84266621131829</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>526.88739348644356</v>
+      </c>
+      <c r="B17">
+        <v>180.83266592418224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>596.63386204558617</v>
+      </c>
+      <c r="B18">
+        <v>187.00643948272096</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>676.14351949012485</v>
+      </c>
+      <c r="B19">
+        <v>192.02716081773431</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>766.98253451320784</v>
+      </c>
+      <c r="B20">
+        <v>195.46591381996029</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>870.99930250701914</v>
+      </c>
+      <c r="B21">
+        <v>196.77789127236366</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>